<commit_message>
editando archivo excel desde el master
</commit_message>
<xml_diff>
--- a/Ex1.xlsx
+++ b/Ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANA\Desktop\ReposGITs\repo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB922C-2629-4969-AC16-0B10833398A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1D8D9F-6DED-4C9F-9C96-2EE7A4D5CDC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5475" yWindow="2175" windowWidth="12885" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
editando el archivo excel desde el master
</commit_message>
<xml_diff>
--- a/Ex1.xlsx
+++ b/Ex1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANA\Desktop\ReposGITs\repo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB922C-2629-4969-AC16-0B10833398A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF66999C-EC5F-497A-996F-17DA417C3834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5475" yWindow="2175" windowWidth="12885" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>